<commit_message>
Added Misc distro grid upload page
</commit_message>
<xml_diff>
--- a/import_templates/Distribution_Grid_Template.xlsx
+++ b/import_templates/Distribution_Grid_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Randy_JR_Stuff\Python_code\chainsight\ChainSight_v2\import_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{116DB156-764B-4A44-BB61-BA1A064B27AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5CCBB2-3470-4E4D-B695-EBCF78610561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distribution_Grid_Template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>STORE_NAME</t>
   </si>
@@ -43,9 +43,6 @@
     <t>SEGMENT</t>
   </si>
   <si>
-    <t>YES_NO</t>
-  </si>
-  <si>
     <t>ACTIVATION_STATUS</t>
   </si>
   <si>
@@ -64,41 +61,23 @@
     <t>HARD BEVERAGES</t>
   </si>
   <si>
-    <t>Cayman Jack Variety 12/12C</t>
-  </si>
-  <si>
-    <t>Guinness Stout 6/12B</t>
-  </si>
-  <si>
-    <t>Diageo</t>
-  </si>
-  <si>
-    <t>IMPORT</t>
-  </si>
-  <si>
-    <t>Angry Orchard Crisp Apple 6/12B</t>
-  </si>
-  <si>
-    <t>Boston Beer</t>
-  </si>
-  <si>
-    <t>CRAFT</t>
-  </si>
-  <si>
-    <t>Twisted Tea Original 12/12C</t>
-  </si>
-  <si>
     <t>Some Store</t>
   </si>
   <si>
     <t>Some Chain</t>
+  </si>
+  <si>
+    <t>Manditory Field</t>
+  </si>
+  <si>
+    <t>YES NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +212,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +399,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -575,8 +574,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -931,14 +932,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -963,21 +974,21 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>2571</v>
@@ -989,135 +1000,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>2571</v>
-      </c>
-      <c r="C4">
-        <v>81582901153</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
-        <v>2571</v>
-      </c>
-      <c r="C5">
-        <v>8382012393</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>2571</v>
-      </c>
-      <c r="C6">
-        <v>8769282102</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>2571</v>
-      </c>
-      <c r="C7">
-        <v>8769283134</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>23</v>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rolled out new secure model
</commit_message>
<xml_diff>
--- a/import_templates/Distribution_Grid_Template.xlsx
+++ b/import_templates/Distribution_Grid_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Randy_JR_Stuff\Python_code\chainsight\ChainSight_v2\import_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5CCBB2-3470-4E4D-B695-EBCF78610561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B30B92-BBE9-48BC-ACBE-CD548E43E3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distribution_Grid_Template" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
     <t>Manditory Field</t>
   </si>
   <si>
-    <t>YES NO</t>
+    <t>YES_NO</t>
   </si>
 </sst>
 </file>
@@ -933,7 +933,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -951,88 +951,88 @@
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>2571</v>
+      </c>
+      <c r="C2">
+        <v>81582901004</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>2571</v>
-      </c>
-      <c r="C3">
-        <v>81582901004</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="H4" s="1" t="s">
+      <c r="E3" s="2"/>
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>